<commit_message>
Work in user v1
</commit_message>
<xml_diff>
--- a/backend/data/tickets.xlsx
+++ b/backend/data/tickets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79109\Desktop\lernin\op_2\project\TravelMaster\backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\komra\Desktop\Бауман\ОП\TravelMaster\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCF2444-3C45-486E-9AFB-1A42D58B60EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -46,12 +47,15 @@
   </si>
   <si>
     <t>RostovSkiRaen</t>
+  </si>
+  <si>
+    <t>2010/12/10/12/35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,16 +411,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -450,10 +454,10 @@
         <v>3000</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -473,7 +477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -493,7 +497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Validation in new tickets
</commit_message>
<xml_diff>
--- a/backend/data/tickets.xlsx
+++ b/backend/data/tickets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,27 +470,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Klg</t>
+          <t>dsada</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RostovSki</t>
+          <t>dsada</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3000</v>
+        <v>333</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10:25</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -501,50 +505,58 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Klg</t>
+          <t>dsada</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>RostovSki</t>
+          <t>sdasdsada</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3000</v>
+        <v>2222</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10:26</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Klg</t>
+          <t>dsada</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>RostovSkiRaen</t>
+          <t>sdasdsada</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3000</v>
+        <v>2221</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>10:28</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -555,23 +567,116 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>dsadasd</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sadasda</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dsada</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>dsadasda</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>dsad</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>asdas</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>2222</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>22:13</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>asdsadas</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dsadasd</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sadasdas</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2001</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>Плацкарт</t>
         </is>

</xml_diff>

<commit_message>
JSON, without basket fixes
</commit_message>
<xml_diff>
--- a/backend/data/tickets.xlsx
+++ b/backend/data/tickets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,24 +475,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dsada</t>
+          <t>Киров</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>dsada</t>
+          <t>Москва</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>333</v>
+        <v>3000</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0:0</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -501,279 +501,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>dsada</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>sdasdsada</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>2222</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>dsada</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>sdasdsada</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>2221</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>dsadasd</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>sadasda</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>dsada</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>dsadasda</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>dsad</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>asdsadas</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>4</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>dsadasd</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>sadasdas</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>2001</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>kaluga</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>peremishl</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>300</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>7:0</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Minsk</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Cheboksary</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>20:0</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begin fix time to string
</commit_message>
<xml_diff>
--- a/backend/data/tickets.xlsx
+++ b/backend/data/tickets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,7 +501,211 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>64</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Калуга</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>600</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1:7</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Калуга</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>700</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Хабаровск</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Хабаровск</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>4500</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>3:2</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Владивосток</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>3700</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3:3</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Плацкарт</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Time fixed and full add JSON
</commit_message>
<xml_diff>
--- a/backend/data/tickets.xlsx
+++ b/backend/data/tickets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,20 +479,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Киров</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
       <c r="E2" t="n">
-        <v>3000</v>
+        <v>2700</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -501,211 +501,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Калуга</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>600</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1:7</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Калуга</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>700</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Хабаровск</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>5000</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Хабаровск</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>4500</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>3:2</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Владивосток</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>3700</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3:3</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0:0</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Плацкарт</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>